<commit_message>
lesson 5 - homework
</commit_message>
<xml_diff>
--- a/Kalenska/Lesson 5 - Test Case/Lession5_automationpractice.xlsx
+++ b/Kalenska/Lesson 5 - Test Case/Lession5_automationpractice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ykalenska2\Desktop\SK04\Kalenska\Lesson 5 - Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE834D-AEA4-47B8-8AF0-E2DEF76694D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DFC28B-5721-4BE1-B879-CD4A832F60D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test case template" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="82">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -105,9 +105,6 @@
 </t>
   </si>
   <si>
-    <t>TC003</t>
-  </si>
-  <si>
     <t>TC004</t>
   </si>
   <si>
@@ -135,18 +132,9 @@
     <t xml:space="preserve">Successful Creation of an Account </t>
   </si>
   <si>
-    <t xml:space="preserve">Enter email address </t>
-  </si>
-  <si>
-    <t>Click "Create an account"</t>
-  </si>
-  <si>
     <t xml:space="preserve">You will be redirected to new page where you need to add your personal information </t>
   </si>
   <si>
-    <t xml:space="preserve">Leave the "Create an Account" field empty </t>
-  </si>
-  <si>
     <t xml:space="preserve">An error message should appear </t>
   </si>
   <si>
@@ -180,9 +168,6 @@
     <t xml:space="preserve">Email: jkalenska@abv.bg / Name: Test / Passowrd: Test1 </t>
   </si>
   <si>
-    <t xml:space="preserve">Unsuccesfull Registration when one of the required fields is not completed </t>
-  </si>
-  <si>
     <t xml:space="preserve">Open the Link </t>
   </si>
   <si>
@@ -243,9 +228,6 @@
     <t>TC008</t>
   </si>
   <si>
-    <t xml:space="preserve">Unsuccesfull redirection to the Registration Page when you leave the email field blank </t>
-  </si>
-  <si>
     <t>TC009</t>
   </si>
   <si>
@@ -256,6 +238,39 @@
   </si>
   <si>
     <t xml:space="preserve">You will be redirected to new page where you need to add your email in order to receive the new passoword </t>
+  </si>
+  <si>
+    <t>Enter email address within the "Create an Account" box</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>You should receive an error message "Ivalid email address"</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave the  "Email Address" field empty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsuccesfull redirection to the Personal Information page when you leave the email field blank </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you try to create an account using the "Sign in" option and you leave the "email address" field blank, you will not be able to proceed with the creation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave the  "Email Address" field within the "Registration" box empty </t>
+  </si>
+  <si>
+    <t>Unsuccesfull redirection to the Personal Information page when you leave add name instead of email address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add name instead of email address within the "Registration" box" box  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsuccesfull Registration when one of the required fields within the Personal Information Page is not completed </t>
   </si>
 </sst>
 </file>
@@ -302,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +327,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -384,6 +417,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,10 +430,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,55 +586,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8832850" y="92075"/>
-          <a:ext cx="1514475" cy="523875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4489450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>908050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>234950</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57D039F7-A108-4EA6-9E78-228744D231F4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8308975" y="92075"/>
           <a:ext cx="1514475" cy="523875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -898,18 +934,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -976,10 +1012,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1025,7 +1061,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,18 +1071,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1061,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1077,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1091,7 +1127,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,10 +1147,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1134,16 +1170,16 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1187,41 +1223,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310021C7-00E5-4035-9F53-CC9B90963EF3}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.28515625" customWidth="1"/>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-    <col min="5" max="5" width="61.85546875" customWidth="1"/>
-    <col min="7" max="7" width="61.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="22" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1230,38 +1264,26 @@
       <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>35</v>
+      <c r="B5" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="23">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1270,70 +1292,50 @@
       <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="22"/>
       <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="G7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>50</v>
+      <c r="B8" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>31</v>
+      <c r="B9" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="E9" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="25">
         <v>43607</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1342,18 +1344,12 @@
       <c r="E10" s="8">
         <v>43607</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="8">
-        <v>43607</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1362,32 +1358,22 @@
       <c r="E11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="26"/>
+      <c r="D12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="G12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1396,123 +1382,318 @@
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="30"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="35">
+        <v>43607</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="36"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="B32" s="39" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="G15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="G17" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="39"/>
+    </row>
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="2" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="32"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="32"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="35">
+        <v>43607</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="36"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="39"/>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>49</v>
+      <c r="B49" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{8A5D5C89-B53F-49B4-9F87-7D19ADBAC2CF}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{A90F62E6-C4A4-400D-82FF-EBE3DF353EAB}"/>
-    <hyperlink ref="H9" r:id="rId3" location="account-creation" xr:uid="{BD26BE71-1263-44C0-AF1F-174BFB99196F}"/>
+    <hyperlink ref="E9" r:id="rId2" location="account-creation" xr:uid="{BD26BE71-1263-44C0-AF1F-174BFB99196F}"/>
+    <hyperlink ref="B27" r:id="rId3" xr:uid="{487533F5-E75F-449C-8F96-5016B198C194}"/>
+    <hyperlink ref="B42" r:id="rId4" xr:uid="{F391B080-A837-48A4-B99A-F9912E70D394}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1520,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6FF86D-AF13-4AFC-9D83-481F8E52A1C7}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,49 +1721,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1590,31 +1771,31 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1676,19 +1857,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>5</v>
@@ -1704,31 +1885,31 @@
         <v>4</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1763,7 +1944,7 @@
         <v>43607</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1796,26 +1977,26 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="G12" s="15" t="s">
+      <c r="E12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="J12" s="15" t="s">
+      <c r="H12" s="17"/>
+      <c r="J12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="15"/>
-      <c r="M12" s="15" t="s">
+      <c r="K12" s="17"/>
+      <c r="M12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N12" s="15"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1881,136 +2062,136 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13"/>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="13"/>
       <c r="G15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="13"/>
       <c r="J15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K15" s="13"/>
       <c r="M15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>57</v>
+      <c r="A19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M12:N12"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:N12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{E77F8C56-2D3E-4633-A28B-0F74F8D21DA4}"/>

</xml_diff>